<commit_message>
filled in much data set
</commit_message>
<xml_diff>
--- a/Data/michigantrees_sequence.xlsx
+++ b/Data/michigantrees_sequence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="540" windowWidth="25040" windowHeight="14260" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="520" windowWidth="25040" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="178">
   <si>
     <t>Family</t>
   </si>
@@ -539,6 +539,21 @@
   </si>
   <si>
     <t>incana_sbsp_rugosa</t>
+  </si>
+  <si>
+    <t>polygamous</t>
+  </si>
+  <si>
+    <t>monoecious/dioecious</t>
+  </si>
+  <si>
+    <t>dioecious/polygamo_monecious</t>
+  </si>
+  <si>
+    <t>polygamo_monecious</t>
+  </si>
+  <si>
+    <t>perfect_or_dioecious</t>
   </si>
 </sst>
 </file>
@@ -927,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2398,8 +2413,11 @@
       <c r="F64">
         <v>16</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>104</v>
       </c>
@@ -2418,8 +2436,11 @@
       <c r="F65">
         <v>26</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>104</v>
       </c>
@@ -2438,8 +2459,11 @@
       <c r="F66">
         <v>22</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>104</v>
       </c>
@@ -2455,8 +2479,14 @@
       <c r="E67" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="F67">
+        <v>25</v>
+      </c>
+      <c r="G67" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>104</v>
       </c>
@@ -2472,8 +2502,14 @@
       <c r="E68" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="F68">
+        <v>25</v>
+      </c>
+      <c r="G68" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>104</v>
       </c>
@@ -2489,8 +2525,14 @@
       <c r="E69" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="F69">
+        <v>18</v>
+      </c>
+      <c r="G69" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>104</v>
       </c>
@@ -2506,8 +2548,14 @@
       <c r="E70" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="F70">
+        <v>28</v>
+      </c>
+      <c r="G70" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>112</v>
       </c>
@@ -2523,8 +2571,14 @@
       <c r="E71" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="F71">
+        <v>30</v>
+      </c>
+      <c r="G71" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>112</v>
       </c>
@@ -2540,8 +2594,14 @@
       <c r="E72" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="F72">
+        <v>18</v>
+      </c>
+      <c r="G72" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>115</v>
       </c>
@@ -2557,8 +2617,14 @@
       <c r="E73" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="F73">
+        <v>20</v>
+      </c>
+      <c r="G73" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>118</v>
       </c>
@@ -2574,8 +2640,14 @@
       <c r="E74" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="F74">
+        <v>7</v>
+      </c>
+      <c r="G74" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>118</v>
       </c>
@@ -2591,8 +2663,14 @@
       <c r="E75" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="F75">
+        <v>9</v>
+      </c>
+      <c r="G75" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>121</v>
       </c>
@@ -2608,8 +2686,14 @@
       <c r="E76" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="F76">
+        <v>27</v>
+      </c>
+      <c r="G76" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>121</v>
       </c>
@@ -2625,8 +2709,14 @@
       <c r="E77" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="F77">
+        <v>30</v>
+      </c>
+      <c r="G77" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>121</v>
       </c>
@@ -2642,8 +2732,14 @@
       <c r="E78" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="F78">
+        <v>30</v>
+      </c>
+      <c r="G78" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>121</v>
       </c>
@@ -2659,8 +2755,14 @@
       <c r="E79" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="F79">
+        <v>30</v>
+      </c>
+      <c r="G79" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>121</v>
       </c>
@@ -2676,8 +2778,14 @@
       <c r="E80" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80">
+        <v>9</v>
+      </c>
+      <c r="G80" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>121</v>
       </c>
@@ -2693,8 +2801,14 @@
       <c r="E81" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>121</v>
       </c>
@@ -2710,8 +2824,14 @@
       <c r="E82" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82">
+        <v>18</v>
+      </c>
+      <c r="G82" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>121</v>
       </c>
@@ -2727,8 +2847,14 @@
       <c r="E83" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83">
+        <v>25</v>
+      </c>
+      <c r="G83" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>121</v>
       </c>
@@ -2744,8 +2870,14 @@
       <c r="E84" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84">
+        <v>15</v>
+      </c>
+      <c r="G84" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>121</v>
       </c>
@@ -2761,8 +2893,14 @@
       <c r="E85" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85">
+        <v>20</v>
+      </c>
+      <c r="G85" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>133</v>
       </c>
@@ -2778,8 +2916,14 @@
       <c r="E86" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86">
+        <v>8</v>
+      </c>
+      <c r="G86" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>133</v>
       </c>
@@ -2795,8 +2939,14 @@
       <c r="E87" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87">
+        <v>10</v>
+      </c>
+      <c r="G87" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>137</v>
       </c>
@@ -2812,8 +2962,14 @@
       <c r="E88" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88">
+        <v>18</v>
+      </c>
+      <c r="G88" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>140</v>
       </c>
@@ -2829,8 +2985,14 @@
       <c r="E89" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89">
+        <v>28</v>
+      </c>
+      <c r="G89" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>140</v>
       </c>
@@ -2846,8 +3008,14 @@
       <c r="E90" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90">
+        <v>20</v>
+      </c>
+      <c r="G90" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>140</v>
       </c>
@@ -2863,8 +3031,14 @@
       <c r="E91" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91">
+        <v>18</v>
+      </c>
+      <c r="G91" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>140</v>
       </c>
@@ -2880,8 +3054,14 @@
       <c r="E92" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92">
+        <v>25</v>
+      </c>
+      <c r="G92" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>140</v>
       </c>
@@ -2897,8 +3077,14 @@
       <c r="E93" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93">
+        <v>15</v>
+      </c>
+      <c r="G93" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>145</v>
       </c>
@@ -2914,8 +3100,14 @@
       <c r="E94" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94">
+        <v>12</v>
+      </c>
+      <c r="G94" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>145</v>
       </c>
@@ -2931,8 +3123,14 @@
       <c r="E95" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95">
+        <v>15</v>
+      </c>
+      <c r="G95" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>149</v>
       </c>
@@ -2947,6 +3145,12 @@
       </c>
       <c r="E96" t="s">
         <v>12</v>
+      </c>
+      <c r="F96">
+        <v>9</v>
+      </c>
+      <c r="G96" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made a source, worked on models
</commit_message>
<xml_diff>
--- a/Data/michigantrees_sequence.xlsx
+++ b/Data/michigantrees_sequence.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="3760" yWindow="4200" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="174">
   <si>
     <t>Family</t>
   </si>
@@ -535,25 +535,13 @@
     <t>polygamo_dioecious</t>
   </si>
   <si>
-    <t>functionially_dioecious</t>
-  </si>
-  <si>
     <t>incana_sbsp_rugosa</t>
   </si>
   <si>
     <t>polygamous</t>
   </si>
   <si>
-    <t>monoecious/dioecious</t>
-  </si>
-  <si>
-    <t>dioecious/polygamo_monecious</t>
-  </si>
-  <si>
     <t>polygamo_monecious</t>
-  </si>
-  <si>
-    <t>perfect_or_dioecious</t>
   </si>
 </sst>
 </file>
@@ -933,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1688,7 +1676,7 @@
         <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -2228,7 +2216,7 @@
         <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D56" t="s">
         <v>21</v>
@@ -2677,7 +2665,7 @@
         <v>27</v>
       </c>
       <c r="G75" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2700,7 +2688,7 @@
         <v>30</v>
       </c>
       <c r="G76" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2723,7 +2711,7 @@
         <v>30</v>
       </c>
       <c r="G77" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2746,7 +2734,7 @@
         <v>30</v>
       </c>
       <c r="G78" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2769,7 +2757,7 @@
         <v>9</v>
       </c>
       <c r="G79" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2815,7 +2803,7 @@
         <v>18</v>
       </c>
       <c r="G81" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2861,7 +2849,7 @@
         <v>15</v>
       </c>
       <c r="G83" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:7">

</xml_diff>

<commit_message>
started adding other categories to data
</commit_message>
<xml_diff>
--- a/Data/michigantrees_sequence.xlsx
+++ b/Data/michigantrees_sequence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="4200" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="3760" yWindow="4200" windowWidth="36860" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="188">
   <si>
     <t>Family</t>
   </si>
@@ -523,9 +523,6 @@
     <t>flower_buds</t>
   </si>
   <si>
-    <t>source</t>
-  </si>
-  <si>
     <t>Gleditsia</t>
   </si>
   <si>
@@ -542,6 +539,51 @@
   </si>
   <si>
     <t>polygamo_monecious</t>
+  </si>
+  <si>
+    <t>shade_tol</t>
+  </si>
+  <si>
+    <t>inflorescence size</t>
+  </si>
+  <si>
+    <t>flower_size</t>
+  </si>
+  <si>
+    <t>intolerant</t>
+  </si>
+  <si>
+    <t>fruit_size</t>
+  </si>
+  <si>
+    <t>5-8</t>
+  </si>
+  <si>
+    <t>5-12</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>tolerant</t>
+  </si>
+  <si>
+    <t>1.5-2</t>
+  </si>
+  <si>
+    <t>1-1.5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>8-10,15-20</t>
   </si>
 </sst>
 </file>
@@ -585,9 +627,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -935,9 +979,10 @@
     <col min="7" max="7" width="19.5" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="11" max="12" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -963,10 +1008,19 @@
         <v>166</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>173</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -988,8 +1042,17 @@
       <c r="G2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="I2" t="s">
+        <v>176</v>
+      </c>
+      <c r="K2" s="3">
+        <v>5</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1011,8 +1074,17 @@
       <c r="G3" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="I3" t="s">
+        <v>183</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1034,8 +1106,17 @@
       <c r="G4" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="I4" t="s">
+        <v>183</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1057,8 +1138,14 @@
       <c r="G5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5" t="s">
+        <v>176</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1080,8 +1167,17 @@
       <c r="G6" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="I6" t="s">
+        <v>183</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1103,8 +1199,14 @@
       <c r="G7" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" t="s">
+        <v>176</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1126,8 +1228,11 @@
       <c r="G8" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1150,7 +1255,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1173,7 +1278,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1196,7 +1301,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1219,7 +1324,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1242,7 +1347,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1265,7 +1370,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1288,7 +1393,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1385,10 +1490,10 @@
         <v>42</v>
       </c>
       <c r="B20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" t="s">
         <v>168</v>
-      </c>
-      <c r="C20" t="s">
-        <v>169</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -1400,7 +1505,7 @@
         <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1423,7 +1528,7 @@
         <v>26</v>
       </c>
       <c r="G21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1860,7 +1965,7 @@
         <v>18</v>
       </c>
       <c r="G40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2216,7 +2321,7 @@
         <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D56" t="s">
         <v>21</v>
@@ -2596,7 +2701,7 @@
         <v>20</v>
       </c>
       <c r="G72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2619,7 +2724,7 @@
         <v>7</v>
       </c>
       <c r="G73" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2642,7 +2747,7 @@
         <v>9</v>
       </c>
       <c r="G74" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2665,7 +2770,7 @@
         <v>27</v>
       </c>
       <c r="G75" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2711,7 +2816,7 @@
         <v>30</v>
       </c>
       <c r="G77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2734,7 +2839,7 @@
         <v>30</v>
       </c>
       <c r="G78" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2757,7 +2862,7 @@
         <v>9</v>
       </c>
       <c r="G79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2849,7 +2954,7 @@
         <v>15</v>
       </c>
       <c r="G83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2941,7 +3046,7 @@
         <v>18</v>
       </c>
       <c r="G87" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2987,7 +3092,7 @@
         <v>20</v>
       </c>
       <c r="G89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" spans="1:7">

</xml_diff>

<commit_message>
began integrating to full data
</commit_message>
<xml_diff>
--- a/Data/michigantrees_sequence.xlsx
+++ b/Data/michigantrees_sequence.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="4200" windowWidth="36860" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="3340" yWindow="140" windowWidth="25600" windowHeight="14760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>Sassafras</t>
   </si>
   <si>
-    <t>albidium</t>
-  </si>
-  <si>
     <t>syn</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>Cercis</t>
   </si>
   <si>
-    <t>candensis</t>
-  </si>
-  <si>
     <t>pro/syn</t>
   </si>
   <si>
@@ -175,9 +169,6 @@
     <t>Rosaceae</t>
   </si>
   <si>
-    <t>Amalanchier</t>
-  </si>
-  <si>
     <t>arborea</t>
   </si>
   <si>
@@ -277,9 +268,6 @@
     <t>macrocarpa</t>
   </si>
   <si>
-    <t xml:space="preserve">Quercus </t>
-  </si>
-  <si>
     <t>muehlenbergii</t>
   </si>
   <si>
@@ -307,12 +295,6 @@
     <t>Betulaceae</t>
   </si>
   <si>
-    <t xml:space="preserve">Alnus </t>
-  </si>
-  <si>
-    <t>gluntinosa</t>
-  </si>
-  <si>
     <t>Betula</t>
   </si>
   <si>
@@ -532,9 +514,6 @@
     <t>polygamo_dioecious</t>
   </si>
   <si>
-    <t>incana_sbsp_rugosa</t>
-  </si>
-  <si>
     <t>polygamous</t>
   </si>
   <si>
@@ -584,6 +563,27 @@
   </si>
   <si>
     <t>8-10,15-20</t>
+  </si>
+  <si>
+    <t>incana</t>
+  </si>
+  <si>
+    <t>Amelanchier</t>
+  </si>
+  <si>
+    <t>Alnus</t>
+  </si>
+  <si>
+    <t>pennsylvanica</t>
+  </si>
+  <si>
+    <t>canadensis</t>
+  </si>
+  <si>
+    <t>glutinosa</t>
+  </si>
+  <si>
+    <t>albidum</t>
   </si>
 </sst>
 </file>
@@ -966,7 +966,7 @@
   <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -999,25 +999,25 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1040,16 +1040,16 @@
         <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="I2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="K2" s="3">
         <v>5</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1072,16 +1072,16 @@
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="I3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1092,132 +1092,132 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>187</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="J4">
         <v>5</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="I6" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I7" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -1226,24 +1226,24 @@
         <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J8" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
       <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
         <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -1252,21 +1252,21 @@
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -1275,21 +1275,21 @@
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -1298,21 +1298,21 @@
         <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -1321,21 +1321,21 @@
         <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -1344,21 +1344,21 @@
         <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -1367,156 +1367,156 @@
         <v>18</v>
       </c>
       <c r="G14" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
         <v>38</v>
       </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15">
         <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>39</v>
-      </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
         <v>38</v>
       </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
-      </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17">
         <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" t="s">
-        <v>39</v>
-      </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18">
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>185</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F19">
         <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C20" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F20">
         <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -1528,18 +1528,18 @@
         <v>26</v>
       </c>
       <c r="G21" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -1551,41 +1551,41 @@
         <v>18</v>
       </c>
       <c r="G22" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>182</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F23">
         <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
         <v>50</v>
       </c>
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -1597,41 +1597,41 @@
         <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25">
         <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -1643,18 +1643,18 @@
         <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -1666,87 +1666,87 @@
         <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F28">
         <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F29">
         <v>25</v>
       </c>
       <c r="G29" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F30">
         <v>10</v>
       </c>
       <c r="G30" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -1758,44 +1758,44 @@
         <v>18</v>
       </c>
       <c r="G31" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F32">
         <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
@@ -1804,21 +1804,21 @@
         <v>30</v>
       </c>
       <c r="G33" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -1827,21 +1827,21 @@
         <v>22</v>
       </c>
       <c r="G34" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" t="s">
-        <v>69</v>
-      </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
@@ -1850,21 +1850,21 @@
         <v>24</v>
       </c>
       <c r="G35" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
@@ -1873,67 +1873,67 @@
         <v>26</v>
       </c>
       <c r="G36" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F37">
         <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F38">
         <v>6</v>
       </c>
       <c r="G38" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1942,67 +1942,67 @@
         <v>18</v>
       </c>
       <c r="G39" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="s">
         <v>73</v>
       </c>
-      <c r="B40" t="s">
-        <v>76</v>
-      </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F40">
         <v>18</v>
       </c>
       <c r="G40" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" t="s">
         <v>73</v>
       </c>
-      <c r="B41" t="s">
-        <v>76</v>
-      </c>
       <c r="C41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F41">
         <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -2011,320 +2011,320 @@
         <v>30</v>
       </c>
       <c r="G42" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" t="s">
         <v>77</v>
       </c>
-      <c r="B43" t="s">
-        <v>80</v>
-      </c>
       <c r="C43" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F43">
         <v>28</v>
       </c>
       <c r="G43" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F44">
         <v>28</v>
       </c>
       <c r="G44" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F45">
         <v>24</v>
       </c>
       <c r="G45" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F46">
         <v>26</v>
       </c>
       <c r="G46" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F47">
         <v>25</v>
       </c>
       <c r="G47" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F48">
         <v>4</v>
       </c>
       <c r="G48" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F49">
         <v>28</v>
       </c>
       <c r="G49" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F50">
         <v>28</v>
       </c>
       <c r="G50" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E51" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F51">
         <v>24</v>
       </c>
       <c r="G51" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B52" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F52">
         <v>21</v>
       </c>
       <c r="G52" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F53">
         <v>18</v>
       </c>
       <c r="G53" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F54">
         <v>20</v>
       </c>
       <c r="G54" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E55" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F55">
         <v>21</v>
       </c>
       <c r="G55" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B56" t="s">
-        <v>95</v>
+        <v>183</v>
       </c>
       <c r="C56" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E56" t="s">
         <v>13</v>
@@ -2333,44 +2333,44 @@
         <v>8</v>
       </c>
       <c r="G56" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
+        <v>183</v>
       </c>
       <c r="C57" t="s">
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="D57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E57" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F57">
         <v>18</v>
       </c>
       <c r="G57" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B58" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C58" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E58" t="s">
         <v>13</v>
@@ -2379,271 +2379,271 @@
         <v>30</v>
       </c>
       <c r="G58" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B59" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C59" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E59" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F59">
         <v>22</v>
       </c>
       <c r="G59" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" t="s">
         <v>94</v>
       </c>
-      <c r="B60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" t="s">
-        <v>100</v>
-      </c>
       <c r="D60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E60" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F60">
         <v>15</v>
       </c>
       <c r="G60" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B61" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E61" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F61">
         <v>18</v>
       </c>
       <c r="G61" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B62" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C62" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F62">
         <v>10</v>
       </c>
       <c r="G62" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B63" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E63" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F63">
         <v>16</v>
       </c>
       <c r="G63" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C64" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E64" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F64">
         <v>26</v>
       </c>
       <c r="G64" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B65" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C65" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F65">
         <v>22</v>
       </c>
       <c r="G65" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B66" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C66" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E66" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F66">
         <v>25</v>
       </c>
       <c r="G66" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C67" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E67" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F67">
         <v>25</v>
       </c>
       <c r="G67" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
+        <v>98</v>
+      </c>
+      <c r="B68" t="s">
         <v>104</v>
       </c>
-      <c r="B68" t="s">
-        <v>110</v>
-      </c>
       <c r="C68" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F68">
         <v>18</v>
       </c>
       <c r="G68" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
+        <v>98</v>
+      </c>
+      <c r="B69" t="s">
         <v>104</v>
       </c>
-      <c r="B69" t="s">
-        <v>110</v>
-      </c>
       <c r="C69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F69">
         <v>28</v>
       </c>
       <c r="G69" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B70" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C70" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
@@ -2655,18 +2655,18 @@
         <v>30</v>
       </c>
       <c r="G70" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B71" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C71" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
@@ -2678,18 +2678,18 @@
         <v>18</v>
       </c>
       <c r="G71" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C72" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D72" t="s">
         <v>11</v>
@@ -2701,18 +2701,18 @@
         <v>20</v>
       </c>
       <c r="G72" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D73" t="s">
         <v>11</v>
@@ -2724,18 +2724,18 @@
         <v>7</v>
       </c>
       <c r="G73" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C74" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D74" t="s">
         <v>11</v>
@@ -2747,67 +2747,67 @@
         <v>9</v>
       </c>
       <c r="G74" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C75" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F75">
         <v>27</v>
       </c>
       <c r="G75" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B76" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C76" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F76">
         <v>30</v>
       </c>
       <c r="G76" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C77" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D77" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E77" t="s">
         <v>13</v>
@@ -2816,21 +2816,21 @@
         <v>30</v>
       </c>
       <c r="G77" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B78" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C78" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D78" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E78" t="s">
         <v>13</v>
@@ -2839,21 +2839,21 @@
         <v>30</v>
       </c>
       <c r="G78" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
+        <v>115</v>
+      </c>
+      <c r="B79" t="s">
+        <v>116</v>
+      </c>
+      <c r="C79" t="s">
         <v>121</v>
       </c>
-      <c r="B79" t="s">
-        <v>122</v>
-      </c>
-      <c r="C79" t="s">
-        <v>127</v>
-      </c>
       <c r="D79" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E79" t="s">
         <v>12</v>
@@ -2862,87 +2862,87 @@
         <v>9</v>
       </c>
       <c r="G79" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B80" t="s">
+        <v>116</v>
+      </c>
+      <c r="C80" t="s">
         <v>122</v>
       </c>
-      <c r="C80" t="s">
-        <v>128</v>
-      </c>
       <c r="D80" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E80" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F80">
         <v>12</v>
       </c>
       <c r="G80" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B81" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C81" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D81" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E81" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F81">
         <v>18</v>
       </c>
       <c r="G81" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B82" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C82" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D82" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E82" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F82">
         <v>25</v>
       </c>
       <c r="G82" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B83" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C83" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D83" t="s">
         <v>11</v>
@@ -2954,18 +2954,18 @@
         <v>15</v>
       </c>
       <c r="G83" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B84" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C84" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
@@ -2977,18 +2977,18 @@
         <v>20</v>
       </c>
       <c r="G84" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B85" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C85" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D85" t="s">
         <v>11</v>
@@ -3000,67 +3000,67 @@
         <v>8</v>
       </c>
       <c r="G85" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B86" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C86" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D86" t="s">
         <v>11</v>
       </c>
       <c r="E86" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F86">
         <v>10</v>
       </c>
       <c r="G86" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B87" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C87" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D87" t="s">
         <v>11</v>
       </c>
       <c r="E87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F87">
         <v>18</v>
       </c>
       <c r="G87" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B88" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C88" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E88" t="s">
         <v>13</v>
@@ -3069,21 +3069,21 @@
         <v>28</v>
       </c>
       <c r="G88" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B89" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C89" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E89" t="s">
         <v>13</v>
@@ -3092,67 +3092,67 @@
         <v>20</v>
       </c>
       <c r="G89" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B90" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C90" t="s">
-        <v>59</v>
+        <v>184</v>
       </c>
       <c r="D90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E90" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F90">
         <v>18</v>
       </c>
       <c r="G90" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B91" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C91" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E91" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F91">
         <v>25</v>
       </c>
       <c r="G91" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B92" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C92" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D92" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E92" t="s">
         <v>13</v>
@@ -3161,18 +3161,18 @@
         <v>15</v>
       </c>
       <c r="G92" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B93" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C93" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D93" t="s">
         <v>11</v>
@@ -3184,18 +3184,18 @@
         <v>12</v>
       </c>
       <c r="G93" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B94" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C94" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D94" t="s">
         <v>11</v>
@@ -3207,18 +3207,18 @@
         <v>15</v>
       </c>
       <c r="G94" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B95" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C95" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D95" t="s">
         <v>11</v>
@@ -3230,7 +3230,7 @@
         <v>9</v>
       </c>
       <c r="G95" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3259,12 +3259,12 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -3272,31 +3272,31 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="C6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added mich_shrubs data to analysis
</commit_message>
<xml_diff>
--- a/Data/michigantrees_sequence.xlsx
+++ b/Data/michigantrees_sequence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="140" windowWidth="25600" windowHeight="14760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="239">
   <si>
     <t>Family</t>
   </si>
@@ -502,9 +502,6 @@
     <t>monoecious</t>
   </si>
   <si>
-    <t>flower_buds</t>
-  </si>
-  <si>
     <t>Gleditsia</t>
   </si>
   <si>
@@ -523,48 +520,12 @@
     <t>shade_tol</t>
   </si>
   <si>
-    <t>inflorescence size</t>
-  </si>
-  <si>
-    <t>flower_size</t>
-  </si>
-  <si>
     <t>intolerant</t>
   </si>
   <si>
-    <t>fruit_size</t>
-  </si>
-  <si>
-    <t>5-8</t>
-  </si>
-  <si>
-    <t>5-12</t>
-  </si>
-  <si>
-    <t>3-4</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2-3</t>
-  </si>
-  <si>
     <t>tolerant</t>
   </si>
   <si>
-    <t>1.5-2</t>
-  </si>
-  <si>
-    <t>1-1.5</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>8-10,15-20</t>
-  </si>
-  <si>
     <t>incana</t>
   </si>
   <si>
@@ -584,6 +545,198 @@
   </si>
   <si>
     <t>albidum</t>
+  </si>
+  <si>
+    <t>av_fruit_time</t>
+  </si>
+  <si>
+    <t>very_intolerant</t>
+  </si>
+  <si>
+    <t>viridus</t>
+  </si>
+  <si>
+    <t>laevis</t>
+  </si>
+  <si>
+    <t>sanguinea</t>
+  </si>
+  <si>
+    <t>Ericaceae</t>
+  </si>
+  <si>
+    <t>Arctostaphylos</t>
+  </si>
+  <si>
+    <t>amomum</t>
+  </si>
+  <si>
+    <t>Corylus</t>
+  </si>
+  <si>
+    <t>cornuta</t>
+  </si>
+  <si>
+    <t>Crataegus</t>
+  </si>
+  <si>
+    <t>chrysocarpa</t>
+  </si>
+  <si>
+    <t>crus-galli</t>
+  </si>
+  <si>
+    <t>macrosperma</t>
+  </si>
+  <si>
+    <t>punctata</t>
+  </si>
+  <si>
+    <t>succulenta</t>
+  </si>
+  <si>
+    <t>Thymelaeaceae</t>
+  </si>
+  <si>
+    <t>Dirca</t>
+  </si>
+  <si>
+    <t>Frangula</t>
+  </si>
+  <si>
+    <t>alnus</t>
+  </si>
+  <si>
+    <t>Aqufoliaceae</t>
+  </si>
+  <si>
+    <t>Ilex</t>
+  </si>
+  <si>
+    <t>mucronata</t>
+  </si>
+  <si>
+    <t>verticillata</t>
+  </si>
+  <si>
+    <t>moderately_tolerant</t>
+  </si>
+  <si>
+    <t>Lindera</t>
+  </si>
+  <si>
+    <t>benzoin</t>
+  </si>
+  <si>
+    <t>Myricaceae</t>
+  </si>
+  <si>
+    <t>Myrica</t>
+  </si>
+  <si>
+    <t>gale</t>
+  </si>
+  <si>
+    <t>Rutaceae</t>
+  </si>
+  <si>
+    <t>Ptelea</t>
+  </si>
+  <si>
+    <t>trifoliata</t>
+  </si>
+  <si>
+    <t>alnifolia</t>
+  </si>
+  <si>
+    <t>aromatica</t>
+  </si>
+  <si>
+    <t>Grossulariaceae</t>
+  </si>
+  <si>
+    <t>Ribes</t>
+  </si>
+  <si>
+    <t>triste</t>
+  </si>
+  <si>
+    <t>bebbiana</t>
+  </si>
+  <si>
+    <t>candida</t>
+  </si>
+  <si>
+    <t>discolor</t>
+  </si>
+  <si>
+    <t>eriocephala</t>
+  </si>
+  <si>
+    <t>interior</t>
+  </si>
+  <si>
+    <t>humilis</t>
+  </si>
+  <si>
+    <t>lucida</t>
+  </si>
+  <si>
+    <t>myricoides</t>
+  </si>
+  <si>
+    <t>pedicellaris</t>
+  </si>
+  <si>
+    <t>petiolaris</t>
+  </si>
+  <si>
+    <t>serissima</t>
+  </si>
+  <si>
+    <t>Elaeagnaceae</t>
+  </si>
+  <si>
+    <t>Shepherdia</t>
+  </si>
+  <si>
+    <t>decora</t>
+  </si>
+  <si>
+    <t>Staphyleaceae</t>
+  </si>
+  <si>
+    <t>Staphylea</t>
+  </si>
+  <si>
+    <t>trifolia</t>
+  </si>
+  <si>
+    <t>Syringa</t>
+  </si>
+  <si>
+    <t>vulgaris</t>
+  </si>
+  <si>
+    <t>Vaccinium</t>
+  </si>
+  <si>
+    <t>myrtilloides</t>
+  </si>
+  <si>
+    <t>ovalifolium</t>
+  </si>
+  <si>
+    <t>pallidum</t>
+  </si>
+  <si>
+    <t>Zanthoxylum</t>
+  </si>
+  <si>
+    <t>americanum</t>
+  </si>
+  <si>
+    <t>uva_ursi</t>
   </si>
 </sst>
 </file>
@@ -627,11 +780,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -979,10 +1130,9 @@
     <col min="7" max="7" width="19.5" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
-    <col min="11" max="12" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,22 +1155,13 @@
         <v>157</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1043,16 +1184,10 @@
         <v>156</v>
       </c>
       <c r="I2" t="s">
-        <v>169</v>
-      </c>
-      <c r="K2" s="3">
-        <v>5</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1075,16 +1210,10 @@
         <v>156</v>
       </c>
       <c r="I3" t="s">
-        <v>176</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1092,7 +1221,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1107,16 +1236,10 @@
         <v>158</v>
       </c>
       <c r="I4" t="s">
-        <v>176</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1139,13 +1262,10 @@
         <v>159</v>
       </c>
       <c r="I5" t="s">
-        <v>169</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1167,17 +1287,14 @@
       <c r="G6" t="s">
         <v>156</v>
       </c>
+      <c r="H6">
+        <v>10.5</v>
+      </c>
       <c r="I6" t="s">
-        <v>176</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1200,13 +1317,10 @@
         <v>159</v>
       </c>
       <c r="I7" t="s">
-        <v>169</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1228,11 +1342,8 @@
       <c r="G8" t="s">
         <v>158</v>
       </c>
-      <c r="J8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1255,7 +1366,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1278,7 +1389,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1301,7 +1412,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1324,7 +1435,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1347,7 +1458,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1370,7 +1481,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1393,7 +1504,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1416,7 +1527,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1439,7 +1550,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1462,7 +1573,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -1470,7 +1581,7 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -1485,15 +1596,15 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>41</v>
       </c>
       <c r="B20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" t="s">
         <v>161</v>
-      </c>
-      <c r="C20" t="s">
-        <v>162</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -1505,10 +1616,10 @@
         <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1528,10 +1639,10 @@
         <v>26</v>
       </c>
       <c r="G21" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1554,12 +1665,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
         <v>49</v>
@@ -1576,8 +1687,14 @@
       <c r="G23" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <v>7</v>
+      </c>
+      <c r="I23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1600,7 +1717,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1623,7 +1740,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1645,8 +1762,14 @@
       <c r="G26" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <v>10</v>
+      </c>
+      <c r="I26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1669,7 +1792,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1692,7 +1815,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -1715,7 +1838,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1738,7 +1861,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1761,7 +1884,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1783,8 +1906,14 @@
       <c r="G32" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32">
+        <v>8.5</v>
+      </c>
+      <c r="I32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -1807,7 +1936,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1830,7 +1959,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -1853,7 +1982,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -1876,7 +2005,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -1899,7 +2028,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -1922,7 +2051,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1945,7 +2074,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -1965,10 +2094,10 @@
         <v>18</v>
       </c>
       <c r="G40" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1991,7 +2120,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -2014,7 +2143,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -2037,7 +2166,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -2060,7 +2189,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -2083,7 +2212,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -2106,7 +2235,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -2129,7 +2258,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>74</v>
       </c>
@@ -2151,8 +2280,11 @@
       <c r="G48" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="I48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -2175,7 +2307,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -2198,7 +2330,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -2221,7 +2353,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>74</v>
       </c>
@@ -2244,7 +2376,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -2267,7 +2399,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -2290,7 +2422,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -2313,15 +2445,15 @@
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>90</v>
       </c>
       <c r="B56" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C56" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="D56" t="s">
         <v>20</v>
@@ -2335,16 +2467,22 @@
       <c r="G56" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56">
+        <v>9</v>
+      </c>
+      <c r="I56" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>90</v>
       </c>
       <c r="B57" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C57" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="D57" t="s">
         <v>20</v>
@@ -2359,7 +2497,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -2382,7 +2520,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -2405,7 +2543,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>90</v>
       </c>
@@ -2428,7 +2566,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>90</v>
       </c>
@@ -2451,7 +2589,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>90</v>
       </c>
@@ -2474,7 +2612,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -2497,7 +2635,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>98</v>
       </c>
@@ -2520,7 +2658,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>98</v>
       </c>
@@ -2543,7 +2681,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>98</v>
       </c>
@@ -2566,7 +2704,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>98</v>
       </c>
@@ -2589,7 +2727,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>98</v>
       </c>
@@ -2612,7 +2750,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>98</v>
       </c>
@@ -2635,7 +2773,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>106</v>
       </c>
@@ -2658,7 +2796,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>106</v>
       </c>
@@ -2681,7 +2819,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>109</v>
       </c>
@@ -2701,10 +2839,10 @@
         <v>20</v>
       </c>
       <c r="G72" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>112</v>
       </c>
@@ -2724,10 +2862,16 @@
         <v>7</v>
       </c>
       <c r="G73" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
+        <v>162</v>
+      </c>
+      <c r="H73">
+        <v>9.5</v>
+      </c>
+      <c r="I73" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>112</v>
       </c>
@@ -2747,10 +2891,16 @@
         <v>9</v>
       </c>
       <c r="G74" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+        <v>162</v>
+      </c>
+      <c r="H74">
+        <v>9.5</v>
+      </c>
+      <c r="I74" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>115</v>
       </c>
@@ -2770,10 +2920,10 @@
         <v>27</v>
       </c>
       <c r="G75" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>115</v>
       </c>
@@ -2796,7 +2946,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>115</v>
       </c>
@@ -2816,10 +2966,10 @@
         <v>30</v>
       </c>
       <c r="G77" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>115</v>
       </c>
@@ -2839,10 +2989,10 @@
         <v>30</v>
       </c>
       <c r="G78" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>115</v>
       </c>
@@ -2853,7 +3003,7 @@
         <v>121</v>
       </c>
       <c r="D79" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E79" t="s">
         <v>12</v>
@@ -2862,10 +3012,16 @@
         <v>9</v>
       </c>
       <c r="G79" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
+        <v>164</v>
+      </c>
+      <c r="H79">
+        <v>7.5</v>
+      </c>
+      <c r="I79" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>115</v>
       </c>
@@ -2876,7 +3032,7 @@
         <v>122</v>
       </c>
       <c r="D80" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E80" t="s">
         <v>58</v>
@@ -2887,8 +3043,14 @@
       <c r="G80" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="81" spans="1:7">
+      <c r="H80">
+        <v>7.5</v>
+      </c>
+      <c r="I80" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>115</v>
       </c>
@@ -2911,7 +3073,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>115</v>
       </c>
@@ -2934,7 +3096,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>115</v>
       </c>
@@ -2954,10 +3116,10 @@
         <v>15</v>
       </c>
       <c r="G83" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>115</v>
       </c>
@@ -2980,7 +3142,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>127</v>
       </c>
@@ -3002,8 +3164,14 @@
       <c r="G85" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="H85">
+        <v>10</v>
+      </c>
+      <c r="I85" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>127</v>
       </c>
@@ -3026,7 +3194,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>131</v>
       </c>
@@ -3046,10 +3214,10 @@
         <v>18</v>
       </c>
       <c r="G87" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>134</v>
       </c>
@@ -3072,7 +3240,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>134</v>
       </c>
@@ -3092,10 +3260,10 @@
         <v>20</v>
       </c>
       <c r="G89" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>134</v>
       </c>
@@ -3103,7 +3271,7 @@
         <v>135</v>
       </c>
       <c r="C90" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D90" t="s">
         <v>20</v>
@@ -3118,7 +3286,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>134</v>
       </c>
@@ -3141,7 +3309,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>134</v>
       </c>
@@ -3164,7 +3332,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>139</v>
       </c>
@@ -3187,7 +3355,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>139</v>
       </c>
@@ -3210,7 +3378,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>143</v>
       </c>
@@ -3227,10 +3395,1283 @@
         <v>12</v>
       </c>
       <c r="F95">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G95" t="s">
         <v>156</v>
+      </c>
+      <c r="H95">
+        <v>9.5</v>
+      </c>
+      <c r="I95" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" t="s">
+        <v>90</v>
+      </c>
+      <c r="B96" t="s">
+        <v>170</v>
+      </c>
+      <c r="C96" t="s">
+        <v>177</v>
+      </c>
+      <c r="D96" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" t="s">
+        <v>16</v>
+      </c>
+      <c r="F96">
+        <v>3</v>
+      </c>
+      <c r="G96" t="s">
+        <v>159</v>
+      </c>
+      <c r="H96">
+        <v>9.5</v>
+      </c>
+      <c r="I96" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" t="s">
+        <v>48</v>
+      </c>
+      <c r="B97" t="s">
+        <v>169</v>
+      </c>
+      <c r="C97" t="s">
+        <v>178</v>
+      </c>
+      <c r="D97" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97" t="s">
+        <v>58</v>
+      </c>
+      <c r="F97">
+        <v>10</v>
+      </c>
+      <c r="G97" t="s">
+        <v>156</v>
+      </c>
+      <c r="H97">
+        <v>7</v>
+      </c>
+      <c r="I97" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>48</v>
+      </c>
+      <c r="B98" t="s">
+        <v>169</v>
+      </c>
+      <c r="C98" t="s">
+        <v>179</v>
+      </c>
+      <c r="D98" t="s">
+        <v>11</v>
+      </c>
+      <c r="E98" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98">
+        <v>8</v>
+      </c>
+      <c r="G98" t="s">
+        <v>156</v>
+      </c>
+      <c r="H98">
+        <v>7</v>
+      </c>
+      <c r="I98" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" t="s">
+        <v>180</v>
+      </c>
+      <c r="B99" t="s">
+        <v>181</v>
+      </c>
+      <c r="C99" t="s">
+        <v>238</v>
+      </c>
+      <c r="D99" t="s">
+        <v>11</v>
+      </c>
+      <c r="E99" t="s">
+        <v>16</v>
+      </c>
+      <c r="F99">
+        <v>0.3</v>
+      </c>
+      <c r="G99" t="s">
+        <v>156</v>
+      </c>
+      <c r="H99">
+        <v>8</v>
+      </c>
+      <c r="I99" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" t="s">
+        <v>127</v>
+      </c>
+      <c r="B100" t="s">
+        <v>128</v>
+      </c>
+      <c r="C100" t="s">
+        <v>182</v>
+      </c>
+      <c r="D100" t="s">
+        <v>11</v>
+      </c>
+      <c r="E100" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100">
+        <v>4</v>
+      </c>
+      <c r="G100" t="s">
+        <v>156</v>
+      </c>
+      <c r="H100">
+        <v>8.5</v>
+      </c>
+      <c r="I100" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" t="s">
+        <v>90</v>
+      </c>
+      <c r="B101" t="s">
+        <v>183</v>
+      </c>
+      <c r="C101" t="s">
+        <v>54</v>
+      </c>
+      <c r="D101" t="s">
+        <v>20</v>
+      </c>
+      <c r="E101" t="s">
+        <v>13</v>
+      </c>
+      <c r="F101">
+        <v>3</v>
+      </c>
+      <c r="G101" t="s">
+        <v>159</v>
+      </c>
+      <c r="H101">
+        <v>8.5</v>
+      </c>
+      <c r="I101" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" t="s">
+        <v>90</v>
+      </c>
+      <c r="B102" t="s">
+        <v>183</v>
+      </c>
+      <c r="C102" t="s">
+        <v>184</v>
+      </c>
+      <c r="D102" t="s">
+        <v>20</v>
+      </c>
+      <c r="E102" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102">
+        <v>4</v>
+      </c>
+      <c r="G102" t="s">
+        <v>159</v>
+      </c>
+      <c r="H102">
+        <v>8.5</v>
+      </c>
+      <c r="I102" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" t="s">
+        <v>48</v>
+      </c>
+      <c r="B103" t="s">
+        <v>185</v>
+      </c>
+      <c r="C103" t="s">
+        <v>186</v>
+      </c>
+      <c r="D103" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" t="s">
+        <v>16</v>
+      </c>
+      <c r="F103">
+        <v>6</v>
+      </c>
+      <c r="G103" t="s">
+        <v>156</v>
+      </c>
+      <c r="H103">
+        <v>9</v>
+      </c>
+      <c r="I103" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" t="s">
+        <v>48</v>
+      </c>
+      <c r="B104" t="s">
+        <v>185</v>
+      </c>
+      <c r="C104" t="s">
+        <v>187</v>
+      </c>
+      <c r="D104" t="s">
+        <v>11</v>
+      </c>
+      <c r="E104" t="s">
+        <v>16</v>
+      </c>
+      <c r="F104">
+        <v>10</v>
+      </c>
+      <c r="G104" t="s">
+        <v>156</v>
+      </c>
+      <c r="H104">
+        <v>9.5</v>
+      </c>
+      <c r="I104" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" t="s">
+        <v>48</v>
+      </c>
+      <c r="B105" t="s">
+        <v>185</v>
+      </c>
+      <c r="C105" t="s">
+        <v>188</v>
+      </c>
+      <c r="D105" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" t="s">
+        <v>16</v>
+      </c>
+      <c r="F105">
+        <v>7</v>
+      </c>
+      <c r="G105" t="s">
+        <v>156</v>
+      </c>
+      <c r="H105">
+        <v>9.5</v>
+      </c>
+      <c r="I105" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" t="s">
+        <v>48</v>
+      </c>
+      <c r="B106" t="s">
+        <v>185</v>
+      </c>
+      <c r="C106" t="s">
+        <v>189</v>
+      </c>
+      <c r="D106" t="s">
+        <v>11</v>
+      </c>
+      <c r="E106" t="s">
+        <v>16</v>
+      </c>
+      <c r="F106">
+        <v>10</v>
+      </c>
+      <c r="G106" t="s">
+        <v>156</v>
+      </c>
+      <c r="H106">
+        <v>8.5</v>
+      </c>
+      <c r="I106" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" t="s">
+        <v>48</v>
+      </c>
+      <c r="B107" t="s">
+        <v>185</v>
+      </c>
+      <c r="C107" t="s">
+        <v>190</v>
+      </c>
+      <c r="D107" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107" t="s">
+        <v>16</v>
+      </c>
+      <c r="F107">
+        <v>8</v>
+      </c>
+      <c r="G107" t="s">
+        <v>156</v>
+      </c>
+      <c r="H107">
+        <v>9.5</v>
+      </c>
+      <c r="I107" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" t="s">
+        <v>191</v>
+      </c>
+      <c r="B108" t="s">
+        <v>192</v>
+      </c>
+      <c r="C108" t="s">
+        <v>88</v>
+      </c>
+      <c r="D108" t="s">
+        <v>11</v>
+      </c>
+      <c r="E108" t="s">
+        <v>13</v>
+      </c>
+      <c r="F108">
+        <v>2</v>
+      </c>
+      <c r="G108" t="s">
+        <v>156</v>
+      </c>
+      <c r="H108">
+        <v>6</v>
+      </c>
+      <c r="I108" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" t="s">
+        <v>60</v>
+      </c>
+      <c r="B109" t="s">
+        <v>193</v>
+      </c>
+      <c r="C109" t="s">
+        <v>194</v>
+      </c>
+      <c r="D109" t="s">
+        <v>11</v>
+      </c>
+      <c r="E109" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109">
+        <v>6</v>
+      </c>
+      <c r="G109" t="s">
+        <v>156</v>
+      </c>
+      <c r="H109">
+        <v>7.5</v>
+      </c>
+      <c r="I109" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" t="s">
+        <v>195</v>
+      </c>
+      <c r="B110" t="s">
+        <v>196</v>
+      </c>
+      <c r="C110" t="s">
+        <v>197</v>
+      </c>
+      <c r="D110" t="s">
+        <v>11</v>
+      </c>
+      <c r="E110" t="s">
+        <v>16</v>
+      </c>
+      <c r="F110">
+        <v>4</v>
+      </c>
+      <c r="G110" t="s">
+        <v>158</v>
+      </c>
+      <c r="H110">
+        <v>7.5</v>
+      </c>
+      <c r="I110" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" t="s">
+        <v>195</v>
+      </c>
+      <c r="B111" t="s">
+        <v>196</v>
+      </c>
+      <c r="C111" t="s">
+        <v>198</v>
+      </c>
+      <c r="D111" t="s">
+        <v>11</v>
+      </c>
+      <c r="E111" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111">
+        <v>5</v>
+      </c>
+      <c r="G111" t="s">
+        <v>158</v>
+      </c>
+      <c r="H111">
+        <v>9.5</v>
+      </c>
+      <c r="I111" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" t="s">
+        <v>14</v>
+      </c>
+      <c r="B112" t="s">
+        <v>200</v>
+      </c>
+      <c r="C112" t="s">
+        <v>201</v>
+      </c>
+      <c r="D112" t="s">
+        <v>11</v>
+      </c>
+      <c r="E112" t="s">
+        <v>13</v>
+      </c>
+      <c r="F112">
+        <v>5</v>
+      </c>
+      <c r="G112" t="s">
+        <v>158</v>
+      </c>
+      <c r="H112">
+        <v>8</v>
+      </c>
+      <c r="I112" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" t="s">
+        <v>202</v>
+      </c>
+      <c r="B113" t="s">
+        <v>203</v>
+      </c>
+      <c r="C113" t="s">
+        <v>204</v>
+      </c>
+      <c r="D113" t="s">
+        <v>20</v>
+      </c>
+      <c r="E113" t="s">
+        <v>13</v>
+      </c>
+      <c r="F113">
+        <v>1.5</v>
+      </c>
+      <c r="G113" t="s">
+        <v>158</v>
+      </c>
+      <c r="H113">
+        <v>7.5</v>
+      </c>
+      <c r="I113" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114" t="s">
+        <v>48</v>
+      </c>
+      <c r="B114" t="s">
+        <v>55</v>
+      </c>
+      <c r="C114" t="s">
+        <v>54</v>
+      </c>
+      <c r="D114" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" t="s">
+        <v>13</v>
+      </c>
+      <c r="F114">
+        <v>10</v>
+      </c>
+      <c r="G114" t="s">
+        <v>156</v>
+      </c>
+      <c r="H114">
+        <v>8.5</v>
+      </c>
+      <c r="I114" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>48</v>
+      </c>
+      <c r="B115" t="s">
+        <v>55</v>
+      </c>
+      <c r="C115" t="s">
+        <v>23</v>
+      </c>
+      <c r="D115" t="s">
+        <v>11</v>
+      </c>
+      <c r="E115" t="s">
+        <v>58</v>
+      </c>
+      <c r="F115">
+        <v>10</v>
+      </c>
+      <c r="G115" t="s">
+        <v>156</v>
+      </c>
+      <c r="H115">
+        <v>7.5</v>
+      </c>
+      <c r="I115" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" t="s">
+        <v>205</v>
+      </c>
+      <c r="B116" t="s">
+        <v>206</v>
+      </c>
+      <c r="C116" t="s">
+        <v>207</v>
+      </c>
+      <c r="D116" t="s">
+        <v>11</v>
+      </c>
+      <c r="E116" t="s">
+        <v>16</v>
+      </c>
+      <c r="F116">
+        <v>5</v>
+      </c>
+      <c r="G116" t="s">
+        <v>163</v>
+      </c>
+      <c r="H116">
+        <v>9.5</v>
+      </c>
+      <c r="I116" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
+        <v>60</v>
+      </c>
+      <c r="B117" t="s">
+        <v>61</v>
+      </c>
+      <c r="C117" t="s">
+        <v>208</v>
+      </c>
+      <c r="D117" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" t="s">
+        <v>16</v>
+      </c>
+      <c r="F117">
+        <v>2</v>
+      </c>
+      <c r="G117" t="s">
+        <v>158</v>
+      </c>
+      <c r="H117">
+        <v>8.5</v>
+      </c>
+      <c r="I117" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" t="s">
+        <v>112</v>
+      </c>
+      <c r="B118" t="s">
+        <v>113</v>
+      </c>
+      <c r="C118" t="s">
+        <v>209</v>
+      </c>
+      <c r="D118" t="s">
+        <v>11</v>
+      </c>
+      <c r="E118" t="s">
+        <v>13</v>
+      </c>
+      <c r="F118">
+        <v>2</v>
+      </c>
+      <c r="G118" t="s">
+        <v>158</v>
+      </c>
+      <c r="H118">
+        <v>7.5</v>
+      </c>
+      <c r="I118" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119" t="s">
+        <v>210</v>
+      </c>
+      <c r="B119" t="s">
+        <v>211</v>
+      </c>
+      <c r="C119" t="s">
+        <v>212</v>
+      </c>
+      <c r="D119" t="s">
+        <v>11</v>
+      </c>
+      <c r="E119" t="s">
+        <v>16</v>
+      </c>
+      <c r="F119">
+        <v>1</v>
+      </c>
+      <c r="G119" t="s">
+        <v>156</v>
+      </c>
+      <c r="H119">
+        <v>7.5</v>
+      </c>
+      <c r="I119" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" t="s">
+        <v>27</v>
+      </c>
+      <c r="B120" t="s">
+        <v>37</v>
+      </c>
+      <c r="C120" t="s">
+        <v>213</v>
+      </c>
+      <c r="D120" t="s">
+        <v>38</v>
+      </c>
+      <c r="E120" t="s">
+        <v>43</v>
+      </c>
+      <c r="F120">
+        <v>4</v>
+      </c>
+      <c r="G120" t="s">
+        <v>158</v>
+      </c>
+      <c r="H120">
+        <v>5.5</v>
+      </c>
+      <c r="I120" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
+        <v>27</v>
+      </c>
+      <c r="B121" t="s">
+        <v>37</v>
+      </c>
+      <c r="C121" t="s">
+        <v>214</v>
+      </c>
+      <c r="D121" t="s">
+        <v>38</v>
+      </c>
+      <c r="E121" t="s">
+        <v>43</v>
+      </c>
+      <c r="F121">
+        <v>1.5</v>
+      </c>
+      <c r="G121" t="s">
+        <v>158</v>
+      </c>
+      <c r="H121">
+        <v>6</v>
+      </c>
+      <c r="I121" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" t="s">
+        <v>27</v>
+      </c>
+      <c r="B122" t="s">
+        <v>37</v>
+      </c>
+      <c r="C122" t="s">
+        <v>108</v>
+      </c>
+      <c r="D122" t="s">
+        <v>38</v>
+      </c>
+      <c r="E122" t="s">
+        <v>43</v>
+      </c>
+      <c r="F122">
+        <v>3</v>
+      </c>
+      <c r="G122" t="s">
+        <v>158</v>
+      </c>
+      <c r="H122">
+        <v>6.5</v>
+      </c>
+      <c r="I122" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" t="s">
+        <v>27</v>
+      </c>
+      <c r="B123" t="s">
+        <v>37</v>
+      </c>
+      <c r="C123" t="s">
+        <v>215</v>
+      </c>
+      <c r="D123" t="s">
+        <v>38</v>
+      </c>
+      <c r="E123" t="s">
+        <v>13</v>
+      </c>
+      <c r="F123">
+        <v>3</v>
+      </c>
+      <c r="G123" t="s">
+        <v>158</v>
+      </c>
+      <c r="H123">
+        <v>5.5</v>
+      </c>
+      <c r="I123" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" t="s">
+        <v>27</v>
+      </c>
+      <c r="B124" t="s">
+        <v>37</v>
+      </c>
+      <c r="C124" t="s">
+        <v>216</v>
+      </c>
+      <c r="D124" t="s">
+        <v>38</v>
+      </c>
+      <c r="E124" t="s">
+        <v>43</v>
+      </c>
+      <c r="F124">
+        <v>6</v>
+      </c>
+      <c r="G124" t="s">
+        <v>158</v>
+      </c>
+      <c r="H124">
+        <v>5.5</v>
+      </c>
+      <c r="I124" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" t="s">
+        <v>27</v>
+      </c>
+      <c r="B125" t="s">
+        <v>37</v>
+      </c>
+      <c r="C125" t="s">
+        <v>217</v>
+      </c>
+      <c r="D125" t="s">
+        <v>38</v>
+      </c>
+      <c r="E125" t="s">
+        <v>16</v>
+      </c>
+      <c r="F125">
+        <v>4</v>
+      </c>
+      <c r="G125" t="s">
+        <v>158</v>
+      </c>
+      <c r="H125">
+        <v>6</v>
+      </c>
+      <c r="I125" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" t="s">
+        <v>27</v>
+      </c>
+      <c r="B126" t="s">
+        <v>37</v>
+      </c>
+      <c r="C126" t="s">
+        <v>218</v>
+      </c>
+      <c r="D126" t="s">
+        <v>38</v>
+      </c>
+      <c r="E126" t="s">
+        <v>13</v>
+      </c>
+      <c r="F126">
+        <v>3</v>
+      </c>
+      <c r="G126" t="s">
+        <v>158</v>
+      </c>
+      <c r="H126">
+        <v>5</v>
+      </c>
+      <c r="I126" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" t="s">
+        <v>27</v>
+      </c>
+      <c r="B127" t="s">
+        <v>37</v>
+      </c>
+      <c r="C127" t="s">
+        <v>219</v>
+      </c>
+      <c r="D127" t="s">
+        <v>38</v>
+      </c>
+      <c r="E127" t="s">
+        <v>16</v>
+      </c>
+      <c r="F127">
+        <v>6</v>
+      </c>
+      <c r="G127" t="s">
+        <v>158</v>
+      </c>
+      <c r="H127">
+        <v>6.5</v>
+      </c>
+      <c r="I127" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128" t="s">
+        <v>27</v>
+      </c>
+      <c r="B128" t="s">
+        <v>37</v>
+      </c>
+      <c r="C128" t="s">
+        <v>220</v>
+      </c>
+      <c r="D128" t="s">
+        <v>38</v>
+      </c>
+      <c r="E128" t="s">
+        <v>43</v>
+      </c>
+      <c r="F128">
+        <v>2.5</v>
+      </c>
+      <c r="G128" t="s">
+        <v>158</v>
+      </c>
+      <c r="H128">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="A129" t="s">
+        <v>27</v>
+      </c>
+      <c r="B129" t="s">
+        <v>37</v>
+      </c>
+      <c r="C129" t="s">
+        <v>221</v>
+      </c>
+      <c r="D129" t="s">
+        <v>38</v>
+      </c>
+      <c r="E129" t="s">
+        <v>16</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="G129" t="s">
+        <v>158</v>
+      </c>
+      <c r="H129">
+        <v>6.5</v>
+      </c>
+      <c r="I129" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="A130" t="s">
+        <v>27</v>
+      </c>
+      <c r="B130" t="s">
+        <v>37</v>
+      </c>
+      <c r="C130" t="s">
+        <v>222</v>
+      </c>
+      <c r="D130" t="s">
+        <v>38</v>
+      </c>
+      <c r="E130" t="s">
+        <v>16</v>
+      </c>
+      <c r="F130">
+        <v>3</v>
+      </c>
+      <c r="G130" t="s">
+        <v>158</v>
+      </c>
+      <c r="I130" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131" t="s">
+        <v>27</v>
+      </c>
+      <c r="B131" t="s">
+        <v>37</v>
+      </c>
+      <c r="C131" t="s">
+        <v>223</v>
+      </c>
+      <c r="D131" t="s">
+        <v>38</v>
+      </c>
+      <c r="E131" t="s">
+        <v>12</v>
+      </c>
+      <c r="F131">
+        <v>4</v>
+      </c>
+      <c r="G131" t="s">
+        <v>158</v>
+      </c>
+      <c r="H131">
+        <v>9</v>
+      </c>
+      <c r="I131" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132" t="s">
+        <v>224</v>
+      </c>
+      <c r="B132" t="s">
+        <v>225</v>
+      </c>
+      <c r="C132" t="s">
+        <v>172</v>
+      </c>
+      <c r="D132" t="s">
+        <v>11</v>
+      </c>
+      <c r="E132" t="s">
+        <v>13</v>
+      </c>
+      <c r="F132">
+        <v>3</v>
+      </c>
+      <c r="G132" t="s">
+        <v>158</v>
+      </c>
+      <c r="H132">
+        <v>7.5</v>
+      </c>
+      <c r="I132" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133" t="s">
+        <v>48</v>
+      </c>
+      <c r="B133" t="s">
+        <v>53</v>
+      </c>
+      <c r="C133" t="s">
+        <v>226</v>
+      </c>
+      <c r="D133" t="s">
+        <v>11</v>
+      </c>
+      <c r="E133" t="s">
+        <v>12</v>
+      </c>
+      <c r="F133">
+        <v>10</v>
+      </c>
+      <c r="G133" t="s">
+        <v>156</v>
+      </c>
+      <c r="H133">
+        <v>8.5</v>
+      </c>
+      <c r="I133" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" t="s">
+        <v>227</v>
+      </c>
+      <c r="B134" t="s">
+        <v>228</v>
+      </c>
+      <c r="C134" t="s">
+        <v>229</v>
+      </c>
+      <c r="D134" t="s">
+        <v>11</v>
+      </c>
+      <c r="E134" t="s">
+        <v>58</v>
+      </c>
+      <c r="F134">
+        <v>4</v>
+      </c>
+      <c r="G134" t="s">
+        <v>156</v>
+      </c>
+      <c r="H134">
+        <v>9.5</v>
+      </c>
+      <c r="I134" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>230</v>
+      </c>
+      <c r="C135" t="s">
+        <v>231</v>
+      </c>
+      <c r="D135" t="s">
+        <v>11</v>
+      </c>
+      <c r="E135" t="s">
+        <v>58</v>
+      </c>
+      <c r="F135">
+        <v>7</v>
+      </c>
+      <c r="G135" t="s">
+        <v>156</v>
+      </c>
+      <c r="I135" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="A136" t="s">
+        <v>180</v>
+      </c>
+      <c r="B136" t="s">
+        <v>232</v>
+      </c>
+      <c r="C136" t="s">
+        <v>233</v>
+      </c>
+      <c r="D136" t="s">
+        <v>11</v>
+      </c>
+      <c r="E136" t="s">
+        <v>16</v>
+      </c>
+      <c r="F136">
+        <v>0.5</v>
+      </c>
+      <c r="G136" t="s">
+        <v>156</v>
+      </c>
+      <c r="H136">
+        <v>7.5</v>
+      </c>
+      <c r="I136" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
+      <c r="A137" t="s">
+        <v>180</v>
+      </c>
+      <c r="B137" t="s">
+        <v>232</v>
+      </c>
+      <c r="C137" t="s">
+        <v>234</v>
+      </c>
+      <c r="D137" t="s">
+        <v>11</v>
+      </c>
+      <c r="E137" t="s">
+        <v>13</v>
+      </c>
+      <c r="F137">
+        <v>1.5</v>
+      </c>
+      <c r="G137" t="s">
+        <v>156</v>
+      </c>
+      <c r="H137">
+        <v>7.5</v>
+      </c>
+      <c r="I137" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
+      <c r="A138" t="s">
+        <v>180</v>
+      </c>
+      <c r="B138" t="s">
+        <v>232</v>
+      </c>
+      <c r="C138" t="s">
+        <v>235</v>
+      </c>
+      <c r="D138" t="s">
+        <v>11</v>
+      </c>
+      <c r="E138" t="s">
+        <v>13</v>
+      </c>
+      <c r="F138">
+        <v>0.8</v>
+      </c>
+      <c r="G138" t="s">
+        <v>156</v>
+      </c>
+      <c r="H138">
+        <v>7.5</v>
+      </c>
+      <c r="I138" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
+      <c r="A139" t="s">
+        <v>205</v>
+      </c>
+      <c r="B139" t="s">
+        <v>236</v>
+      </c>
+      <c r="C139" t="s">
+        <v>237</v>
+      </c>
+      <c r="D139" t="s">
+        <v>11</v>
+      </c>
+      <c r="E139" t="s">
+        <v>13</v>
+      </c>
+      <c r="F139">
+        <v>5</v>
+      </c>
+      <c r="G139" t="s">
+        <v>158</v>
+      </c>
+      <c r="H139">
+        <v>8.5</v>
+      </c>
+      <c r="I139" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated all Mich flora data and models
</commit_message>
<xml_diff>
--- a/Data/michigantrees_sequence.xlsx
+++ b/Data/michigantrees_sequence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="248">
   <si>
     <t>Family</t>
   </si>
@@ -737,6 +737,33 @@
   </si>
   <si>
     <t>uva_ursi</t>
+  </si>
+  <si>
+    <t>very_tolerant</t>
+  </si>
+  <si>
+    <t>av.fruit time</t>
+  </si>
+  <si>
+    <t>1-12=Jan-Dec</t>
+  </si>
+  <si>
+    <t>autmn=9.5</t>
+  </si>
+  <si>
+    <t>late autumn=10</t>
+  </si>
+  <si>
+    <t>early autmn=9</t>
+  </si>
+  <si>
+    <t>very intolerant</t>
+  </si>
+  <si>
+    <t>moderately tolerant</t>
+  </si>
+  <si>
+    <t>very tolerant</t>
   </si>
 </sst>
 </file>
@@ -1116,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1183,6 +1210,9 @@
       <c r="G2" t="s">
         <v>156</v>
       </c>
+      <c r="H2">
+        <v>9.5</v>
+      </c>
       <c r="I2" t="s">
         <v>166</v>
       </c>
@@ -1209,6 +1239,9 @@
       <c r="G3" t="s">
         <v>156</v>
       </c>
+      <c r="H3">
+        <v>9.5</v>
+      </c>
       <c r="I3" t="s">
         <v>167</v>
       </c>
@@ -1235,6 +1268,9 @@
       <c r="G4" t="s">
         <v>158</v>
       </c>
+      <c r="H4">
+        <v>9.5</v>
+      </c>
       <c r="I4" t="s">
         <v>167</v>
       </c>
@@ -1261,6 +1297,9 @@
       <c r="G5" t="s">
         <v>159</v>
       </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
       <c r="I5" t="s">
         <v>166</v>
       </c>
@@ -1342,6 +1381,12 @@
       <c r="G8" t="s">
         <v>158</v>
       </c>
+      <c r="H8">
+        <v>5.5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
@@ -1365,6 +1410,9 @@
       <c r="G9" t="s">
         <v>158</v>
       </c>
+      <c r="I9" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
@@ -1388,6 +1436,12 @@
       <c r="G10" t="s">
         <v>158</v>
       </c>
+      <c r="H10">
+        <v>5.5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
@@ -1411,6 +1465,12 @@
       <c r="G11" t="s">
         <v>158</v>
       </c>
+      <c r="H11">
+        <v>5.5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
@@ -1434,6 +1494,12 @@
       <c r="G12" t="s">
         <v>158</v>
       </c>
+      <c r="H12">
+        <v>5.5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
@@ -1457,6 +1523,12 @@
       <c r="G13" t="s">
         <v>158</v>
       </c>
+      <c r="H13">
+        <v>5.5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
@@ -1480,6 +1552,12 @@
       <c r="G14" t="s">
         <v>158</v>
       </c>
+      <c r="H14">
+        <v>5.5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
@@ -1503,6 +1581,12 @@
       <c r="G15" t="s">
         <v>158</v>
       </c>
+      <c r="H15">
+        <v>5.5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
@@ -1526,6 +1610,12 @@
       <c r="G16" t="s">
         <v>158</v>
       </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
@@ -1549,6 +1639,12 @@
       <c r="G17" t="s">
         <v>158</v>
       </c>
+      <c r="H17">
+        <v>5.5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
@@ -1572,6 +1668,12 @@
       <c r="G18" t="s">
         <v>158</v>
       </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
@@ -1595,6 +1697,12 @@
       <c r="G19" t="s">
         <v>156</v>
       </c>
+      <c r="H19">
+        <v>6.5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
@@ -1618,6 +1726,12 @@
       <c r="G20" t="s">
         <v>162</v>
       </c>
+      <c r="H20">
+        <v>9.5</v>
+      </c>
+      <c r="I20" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
@@ -1641,6 +1755,12 @@
       <c r="G21" t="s">
         <v>162</v>
       </c>
+      <c r="H21">
+        <v>9.5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
@@ -1664,6 +1784,12 @@
       <c r="G22" t="s">
         <v>156</v>
       </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
@@ -1716,6 +1842,12 @@
       <c r="G24" t="s">
         <v>156</v>
       </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
@@ -1739,6 +1871,12 @@
       <c r="G25" t="s">
         <v>156</v>
       </c>
+      <c r="H25">
+        <v>8.5</v>
+      </c>
+      <c r="I25" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
@@ -1766,7 +1904,7 @@
         <v>10</v>
       </c>
       <c r="I26" t="s">
-        <v>166</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1791,6 +1929,12 @@
       <c r="G27" t="s">
         <v>156</v>
       </c>
+      <c r="H27">
+        <v>8.5</v>
+      </c>
+      <c r="I27" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
@@ -1814,6 +1958,12 @@
       <c r="G28" t="s">
         <v>156</v>
       </c>
+      <c r="H28">
+        <v>7.5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
@@ -1837,6 +1987,12 @@
       <c r="G29" t="s">
         <v>156</v>
       </c>
+      <c r="H29">
+        <v>8.5</v>
+      </c>
+      <c r="I29" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
@@ -1860,6 +2016,12 @@
       <c r="G30" t="s">
         <v>156</v>
       </c>
+      <c r="H30">
+        <v>7.5</v>
+      </c>
+      <c r="I30" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
@@ -1883,6 +2045,12 @@
       <c r="G31" t="s">
         <v>156</v>
       </c>
+      <c r="H31">
+        <v>8.5</v>
+      </c>
+      <c r="I31" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
@@ -1935,6 +2103,12 @@
       <c r="G33" t="s">
         <v>156</v>
       </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+      <c r="I33" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
@@ -1958,6 +2132,12 @@
       <c r="G34" t="s">
         <v>156</v>
       </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+      <c r="I34" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
@@ -1981,6 +2161,12 @@
       <c r="G35" t="s">
         <v>156</v>
       </c>
+      <c r="H35">
+        <v>5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
@@ -2004,6 +2190,12 @@
       <c r="G36" t="s">
         <v>156</v>
       </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
@@ -2027,6 +2219,12 @@
       <c r="G37" t="s">
         <v>159</v>
       </c>
+      <c r="H37">
+        <v>9.5</v>
+      </c>
+      <c r="I37" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
@@ -2050,6 +2248,12 @@
       <c r="G38" t="s">
         <v>159</v>
       </c>
+      <c r="H38">
+        <v>9</v>
+      </c>
+      <c r="I38" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
@@ -2073,6 +2277,12 @@
       <c r="G39" t="s">
         <v>158</v>
       </c>
+      <c r="H39">
+        <v>9.5</v>
+      </c>
+      <c r="I39" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
@@ -2096,6 +2306,12 @@
       <c r="G40" t="s">
         <v>162</v>
       </c>
+      <c r="H40">
+        <v>6.5</v>
+      </c>
+      <c r="I40" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
@@ -2119,6 +2335,12 @@
       <c r="G41" t="s">
         <v>158</v>
       </c>
+      <c r="H41">
+        <v>7</v>
+      </c>
+      <c r="I41" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
@@ -2142,6 +2364,12 @@
       <c r="G42" t="s">
         <v>159</v>
       </c>
+      <c r="H42">
+        <v>9.5</v>
+      </c>
+      <c r="I42" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
@@ -2165,6 +2393,12 @@
       <c r="G43" t="s">
         <v>159</v>
       </c>
+      <c r="H43">
+        <v>9.5</v>
+      </c>
+      <c r="I43" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
@@ -2188,6 +2422,12 @@
       <c r="G44" t="s">
         <v>159</v>
       </c>
+      <c r="H44">
+        <v>9.5</v>
+      </c>
+      <c r="I44" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
@@ -2211,6 +2451,12 @@
       <c r="G45" t="s">
         <v>159</v>
       </c>
+      <c r="H45">
+        <v>9.5</v>
+      </c>
+      <c r="I45" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
@@ -2234,6 +2480,12 @@
       <c r="G46" t="s">
         <v>159</v>
       </c>
+      <c r="H46">
+        <v>9.5</v>
+      </c>
+      <c r="I46" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
@@ -2257,6 +2509,12 @@
       <c r="G47" t="s">
         <v>159</v>
       </c>
+      <c r="H47">
+        <v>9.5</v>
+      </c>
+      <c r="I47" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
@@ -2280,6 +2538,9 @@
       <c r="G48" t="s">
         <v>159</v>
       </c>
+      <c r="H48">
+        <v>19</v>
+      </c>
       <c r="I48" t="s">
         <v>166</v>
       </c>
@@ -2306,6 +2567,12 @@
       <c r="G49" t="s">
         <v>159</v>
       </c>
+      <c r="H49">
+        <v>19</v>
+      </c>
+      <c r="I49" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
@@ -2329,6 +2596,12 @@
       <c r="G50" t="s">
         <v>159</v>
       </c>
+      <c r="H50">
+        <v>19</v>
+      </c>
+      <c r="I50" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
@@ -2352,6 +2625,12 @@
       <c r="G51" t="s">
         <v>159</v>
       </c>
+      <c r="H51">
+        <v>19</v>
+      </c>
+      <c r="I51" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
@@ -2375,6 +2654,12 @@
       <c r="G52" t="s">
         <v>159</v>
       </c>
+      <c r="H52">
+        <v>19</v>
+      </c>
+      <c r="I52" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
@@ -2398,6 +2683,12 @@
       <c r="G53" t="s">
         <v>159</v>
       </c>
+      <c r="H53">
+        <v>19</v>
+      </c>
+      <c r="I53" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
@@ -2421,6 +2712,12 @@
       <c r="G54" t="s">
         <v>159</v>
       </c>
+      <c r="H54">
+        <v>19</v>
+      </c>
+      <c r="I54" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
@@ -2444,6 +2741,12 @@
       <c r="G55" t="s">
         <v>159</v>
       </c>
+      <c r="H55">
+        <v>19</v>
+      </c>
+      <c r="I55" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
@@ -2496,6 +2799,12 @@
       <c r="G57" t="s">
         <v>159</v>
       </c>
+      <c r="H57">
+        <v>9.5</v>
+      </c>
+      <c r="I57" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
@@ -2519,6 +2828,12 @@
       <c r="G58" t="s">
         <v>159</v>
       </c>
+      <c r="H58">
+        <v>8</v>
+      </c>
+      <c r="I58" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
@@ -2542,6 +2857,12 @@
       <c r="G59" t="s">
         <v>159</v>
       </c>
+      <c r="H59">
+        <v>8.5</v>
+      </c>
+      <c r="I59" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
@@ -2565,6 +2886,12 @@
       <c r="G60" t="s">
         <v>159</v>
       </c>
+      <c r="H60">
+        <v>8.5</v>
+      </c>
+      <c r="I60" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
@@ -2588,6 +2915,12 @@
       <c r="G61" t="s">
         <v>159</v>
       </c>
+      <c r="H61">
+        <v>5.5</v>
+      </c>
+      <c r="I61" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
@@ -2611,6 +2944,12 @@
       <c r="G62" t="s">
         <v>159</v>
       </c>
+      <c r="H62">
+        <v>6</v>
+      </c>
+      <c r="I62" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
@@ -2634,6 +2973,12 @@
       <c r="G63" t="s">
         <v>159</v>
       </c>
+      <c r="H63">
+        <v>9</v>
+      </c>
+      <c r="I63" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
@@ -2657,6 +3002,12 @@
       <c r="G64" t="s">
         <v>159</v>
       </c>
+      <c r="H64">
+        <v>10</v>
+      </c>
+      <c r="I64" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
@@ -2680,6 +3031,12 @@
       <c r="G65" t="s">
         <v>159</v>
       </c>
+      <c r="H65">
+        <v>10</v>
+      </c>
+      <c r="I65" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
@@ -2703,6 +3060,12 @@
       <c r="G66" t="s">
         <v>159</v>
       </c>
+      <c r="H66">
+        <v>10</v>
+      </c>
+      <c r="I66" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
@@ -2726,6 +3089,12 @@
       <c r="G67" t="s">
         <v>159</v>
       </c>
+      <c r="H67">
+        <v>10</v>
+      </c>
+      <c r="I67" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
@@ -2749,6 +3118,12 @@
       <c r="G68" t="s">
         <v>159</v>
       </c>
+      <c r="H68">
+        <v>10</v>
+      </c>
+      <c r="I68" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
@@ -2772,6 +3147,12 @@
       <c r="G69" t="s">
         <v>159</v>
       </c>
+      <c r="H69">
+        <v>10</v>
+      </c>
+      <c r="I69" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
@@ -2795,6 +3176,12 @@
       <c r="G70" t="s">
         <v>156</v>
       </c>
+      <c r="H70">
+        <v>10</v>
+      </c>
+      <c r="I70" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
@@ -2818,6 +3205,12 @@
       <c r="G71" t="s">
         <v>156</v>
       </c>
+      <c r="H71">
+        <v>10</v>
+      </c>
+      <c r="I71" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
@@ -2841,6 +3234,12 @@
       <c r="G72" t="s">
         <v>162</v>
       </c>
+      <c r="H72">
+        <v>10</v>
+      </c>
+      <c r="I72" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
@@ -2922,6 +3321,12 @@
       <c r="G75" t="s">
         <v>163</v>
       </c>
+      <c r="H75">
+        <v>10</v>
+      </c>
+      <c r="I75" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
@@ -2945,6 +3350,12 @@
       <c r="G76" t="s">
         <v>159</v>
       </c>
+      <c r="H76">
+        <v>9.5</v>
+      </c>
+      <c r="I76" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
@@ -2957,7 +3368,7 @@
         <v>119</v>
       </c>
       <c r="D77" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E77" t="s">
         <v>13</v>
@@ -2967,6 +3378,12 @@
       </c>
       <c r="G77" t="s">
         <v>164</v>
+      </c>
+      <c r="H77">
+        <v>5.5</v>
+      </c>
+      <c r="I77" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -2980,7 +3397,7 @@
         <v>120</v>
       </c>
       <c r="D78" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E78" t="s">
         <v>13</v>
@@ -2990,6 +3407,12 @@
       </c>
       <c r="G78" t="s">
         <v>164</v>
+      </c>
+      <c r="H78">
+        <v>5</v>
+      </c>
+      <c r="I78" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -3061,7 +3484,7 @@
         <v>123</v>
       </c>
       <c r="D81" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E81" t="s">
         <v>43</v>
@@ -3071,6 +3494,12 @@
       </c>
       <c r="G81" t="s">
         <v>158</v>
+      </c>
+      <c r="H81">
+        <v>9.5</v>
+      </c>
+      <c r="I81" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3084,7 +3513,7 @@
         <v>124</v>
       </c>
       <c r="D82" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E82" t="s">
         <v>43</v>
@@ -3094,6 +3523,12 @@
       </c>
       <c r="G82" t="s">
         <v>158</v>
+      </c>
+      <c r="H82">
+        <v>9.5</v>
+      </c>
+      <c r="I82" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3118,6 +3553,12 @@
       <c r="G83" t="s">
         <v>164</v>
       </c>
+      <c r="H83">
+        <v>10</v>
+      </c>
+      <c r="I83" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
@@ -3139,7 +3580,13 @@
         <v>20</v>
       </c>
       <c r="G84" t="s">
-        <v>31</v>
+        <v>156</v>
+      </c>
+      <c r="H84">
+        <v>10</v>
+      </c>
+      <c r="I84" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3193,6 +3640,12 @@
       <c r="G86" t="s">
         <v>156</v>
       </c>
+      <c r="H86">
+        <v>10</v>
+      </c>
+      <c r="I86" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
@@ -3216,6 +3669,12 @@
       <c r="G87" t="s">
         <v>162</v>
       </c>
+      <c r="H87">
+        <v>10</v>
+      </c>
+      <c r="I87" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
@@ -3239,6 +3698,12 @@
       <c r="G88" t="s">
         <v>158</v>
       </c>
+      <c r="H88">
+        <v>8.5</v>
+      </c>
+      <c r="I88" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
@@ -3262,6 +3727,12 @@
       <c r="G89" t="s">
         <v>162</v>
       </c>
+      <c r="H89">
+        <v>8.5</v>
+      </c>
+      <c r="I89" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
@@ -3285,6 +3756,12 @@
       <c r="G90" t="s">
         <v>158</v>
       </c>
+      <c r="H90">
+        <v>9</v>
+      </c>
+      <c r="I90" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
@@ -3308,6 +3785,12 @@
       <c r="G91" t="s">
         <v>158</v>
       </c>
+      <c r="H91">
+        <v>9</v>
+      </c>
+      <c r="I91" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
@@ -3331,6 +3814,12 @@
       <c r="G92" t="s">
         <v>156</v>
       </c>
+      <c r="H92">
+        <v>9.5</v>
+      </c>
+      <c r="I92" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
@@ -3354,6 +3843,12 @@
       <c r="G93" t="s">
         <v>156</v>
       </c>
+      <c r="H93">
+        <v>9</v>
+      </c>
+      <c r="I93" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
@@ -3376,6 +3871,12 @@
       </c>
       <c r="G94" t="s">
         <v>156</v>
+      </c>
+      <c r="H94">
+        <v>9</v>
+      </c>
+      <c r="I94" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -4686,10 +5187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4698,46 +5199,81 @@
     <col min="3" max="3" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="B2" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>148</v>
       </c>
       <c r="C3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>149</v>
       </c>
       <c r="C4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>150</v>
       </c>
       <c r="C5" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="C6" t="s">
         <v>154</v>
+      </c>
+      <c r="D6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="E7" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>